<commit_message>
Fix expected xlsx for exportServiceIT
</commit_message>
<xml_diff>
--- a/molgenis-platform-integration-tests/src/test/resources/xls/expectedDownloadResult.xlsx
+++ b/molgenis-platform-integration-tests/src/test/resources/xls/expectedDownloadResult.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bart\Documents\GitHub\molgenis\molgenis-platform-integration-tests\src\test\resources\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17492FE1-C882-47D3-B9CB-1D5C5019719E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D20DDC6-25AD-41A2-A810-EB318D1D41CA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="96">
   <si>
     <t>name</t>
   </si>
@@ -286,6 +286,12 @@
   </si>
   <si>
     <t>string1</t>
+  </si>
+  <si>
+    <t>2012-12-21</t>
+  </si>
+  <si>
+    <t>1985-08-12T08:12:13+0200</t>
   </si>
   <si>
     <t>this.is@mail.address</t>
@@ -688,12 +694,6 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
       <c r="E2" t="s">
         <v>6</v>
       </c>
@@ -705,9 +705,6 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
@@ -721,12 +718,6 @@
       </c>
       <c r="B4" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
@@ -744,13 +735,6 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -974,9 +958,6 @@
       <c r="N2" t="s">
         <v>15</v>
       </c>
-      <c r="O2" t="s">
-        <v>6</v>
-      </c>
       <c r="W2" t="s">
         <v>6</v>
       </c>
@@ -1015,9 +996,6 @@
       <c r="N3" t="s">
         <v>15</v>
       </c>
-      <c r="O3" t="s">
-        <v>6</v>
-      </c>
       <c r="W3" t="s">
         <v>6</v>
       </c>
@@ -1056,9 +1034,6 @@
       <c r="N4" t="s">
         <v>15</v>
       </c>
-      <c r="O4" t="s">
-        <v>6</v>
-      </c>
       <c r="W4" t="s">
         <v>6</v>
       </c>
@@ -1097,9 +1072,6 @@
       <c r="N5" t="s">
         <v>15</v>
       </c>
-      <c r="O5" t="s">
-        <v>6</v>
-      </c>
       <c r="W5" t="s">
         <v>6</v>
       </c>
@@ -1135,9 +1107,6 @@
       <c r="N6" t="s">
         <v>15</v>
       </c>
-      <c r="O6" t="s">
-        <v>6</v>
-      </c>
       <c r="V6" t="s">
         <v>41</v>
       </c>
@@ -1179,9 +1148,6 @@
       <c r="N7" t="s">
         <v>15</v>
       </c>
-      <c r="O7" t="s">
-        <v>6</v>
-      </c>
       <c r="W7" t="s">
         <v>6</v>
       </c>
@@ -1220,9 +1186,6 @@
       <c r="N8" t="s">
         <v>15</v>
       </c>
-      <c r="O8" t="s">
-        <v>6</v>
-      </c>
       <c r="W8" t="s">
         <v>6</v>
       </c>
@@ -1258,9 +1221,6 @@
       <c r="N9" t="s">
         <v>15</v>
       </c>
-      <c r="O9" t="s">
-        <v>6</v>
-      </c>
       <c r="W9" t="s">
         <v>6</v>
       </c>
@@ -1337,9 +1297,6 @@
       <c r="N11" t="s">
         <v>15</v>
       </c>
-      <c r="O11" t="s">
-        <v>6</v>
-      </c>
       <c r="W11" t="s">
         <v>6</v>
       </c>
@@ -1375,9 +1332,6 @@
       <c r="N12" t="s">
         <v>15</v>
       </c>
-      <c r="O12" t="s">
-        <v>6</v>
-      </c>
       <c r="W12" t="s">
         <v>6</v>
       </c>
@@ -1413,9 +1367,6 @@
       <c r="N13" t="s">
         <v>15</v>
       </c>
-      <c r="O13" t="s">
-        <v>6</v>
-      </c>
       <c r="W13" t="s">
         <v>6</v>
       </c>
@@ -1451,9 +1402,6 @@
       <c r="N14" t="s">
         <v>15</v>
       </c>
-      <c r="O14" t="s">
-        <v>6</v>
-      </c>
       <c r="W14" t="s">
         <v>6</v>
       </c>
@@ -1489,9 +1437,6 @@
       <c r="N15" t="s">
         <v>15</v>
       </c>
-      <c r="O15" t="s">
-        <v>6</v>
-      </c>
       <c r="W15" t="s">
         <v>6</v>
       </c>
@@ -1527,9 +1472,6 @@
       <c r="N16" t="s">
         <v>15</v>
       </c>
-      <c r="O16" t="s">
-        <v>6</v>
-      </c>
       <c r="W16" t="s">
         <v>6</v>
       </c>
@@ -1565,9 +1507,6 @@
       <c r="N17" t="s">
         <v>15</v>
       </c>
-      <c r="O17" t="s">
-        <v>6</v>
-      </c>
       <c r="V17" t="s">
         <v>72</v>
       </c>
@@ -1606,9 +1545,6 @@
       <c r="N18" t="s">
         <v>15</v>
       </c>
-      <c r="O18" t="s">
-        <v>6</v>
-      </c>
       <c r="W18" t="s">
         <v>6</v>
       </c>
@@ -1647,9 +1583,6 @@
       <c r="N19" t="s">
         <v>15</v>
       </c>
-      <c r="O19" t="s">
-        <v>6</v>
-      </c>
       <c r="W19" t="s">
         <v>6</v>
       </c>
@@ -1688,9 +1621,6 @@
       <c r="N20" t="s">
         <v>15</v>
       </c>
-      <c r="O20" t="s">
-        <v>6</v>
-      </c>
       <c r="W20" t="s">
         <v>6</v>
       </c>
@@ -1726,9 +1656,6 @@
       <c r="N21" t="s">
         <v>15</v>
       </c>
-      <c r="O21" t="s">
-        <v>6</v>
-      </c>
       <c r="T21" t="s">
         <v>70</v>
       </c>
@@ -1767,9 +1694,6 @@
       <c r="N22" t="s">
         <v>15</v>
       </c>
-      <c r="O22" t="s">
-        <v>6</v>
-      </c>
       <c r="W22" t="s">
         <v>6</v>
       </c>
@@ -1805,9 +1729,6 @@
       <c r="N23" t="s">
         <v>15</v>
       </c>
-      <c r="O23" t="s">
-        <v>6</v>
-      </c>
       <c r="P23" t="s">
         <v>80</v>
       </c>
@@ -1849,9 +1770,6 @@
       <c r="N24" t="s">
         <v>15</v>
       </c>
-      <c r="O24" t="s">
-        <v>6</v>
-      </c>
       <c r="W24" t="s">
         <v>6</v>
       </c>
@@ -1889,9 +1807,6 @@
       </c>
       <c r="N25" t="s">
         <v>15</v>
-      </c>
-      <c r="O25" t="s">
-        <v>6</v>
       </c>
       <c r="W25" t="s">
         <v>6</v>
@@ -1943,18 +1858,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -2031,23 +1937,23 @@
       <c r="E2" t="s">
         <v>83</v>
       </c>
-      <c r="F2">
-        <v>41264</v>
+      <c r="F2" t="s">
+        <v>87</v>
       </c>
       <c r="G2" t="s">
         <v>57</v>
       </c>
-      <c r="H2">
-        <v>31271.341817129629</v>
+      <c r="H2" t="s">
+        <v>88</v>
       </c>
       <c r="I2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="J2">
         <v>0.123</v>
       </c>
       <c r="L2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -2056,7 +1962,7 @@
         <v>10</v>
       </c>
       <c r="O2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="P2" t="s">
         <v>83</v>
@@ -2084,26 +1990,26 @@
       <c r="E3" t="s">
         <v>72</v>
       </c>
-      <c r="F3">
-        <v>41264</v>
+      <c r="F3" t="s">
+        <v>87</v>
       </c>
       <c r="G3" t="s">
-        <v>90</v>
-      </c>
-      <c r="H3">
-        <v>31271.341817129629</v>
+        <v>92</v>
+      </c>
+      <c r="H3" t="s">
+        <v>88</v>
       </c>
       <c r="I3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="J3">
         <v>1.123</v>
       </c>
       <c r="K3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="M3">
         <v>1000000</v>
@@ -2112,7 +2018,7 @@
         <v>11</v>
       </c>
       <c r="O3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="P3" t="s">
         <v>72</v>
@@ -2126,7 +2032,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
         <v>86</v>
@@ -2140,23 +2046,23 @@
       <c r="E4" t="s">
         <v>83</v>
       </c>
-      <c r="F4">
-        <v>41264</v>
+      <c r="F4" t="s">
+        <v>87</v>
       </c>
       <c r="G4" t="s">
         <v>57</v>
       </c>
-      <c r="H4">
-        <v>31271.341817129629</v>
+      <c r="H4" t="s">
+        <v>88</v>
       </c>
       <c r="I4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="J4">
         <v>2.1230000000000002</v>
       </c>
       <c r="L4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="M4">
         <v>2000000</v>
@@ -2165,7 +2071,7 @@
         <v>12</v>
       </c>
       <c r="O4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="P4" t="s">
         <v>83</v>
@@ -2179,7 +2085,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
         <v>86</v>
@@ -2193,26 +2099,26 @@
       <c r="E5" t="s">
         <v>72</v>
       </c>
-      <c r="F5">
-        <v>41264</v>
+      <c r="F5" t="s">
+        <v>87</v>
       </c>
       <c r="G5" t="s">
-        <v>90</v>
-      </c>
-      <c r="H5">
-        <v>31271.341817129629</v>
+        <v>92</v>
+      </c>
+      <c r="H5" t="s">
+        <v>88</v>
       </c>
       <c r="I5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="J5">
         <v>3.1230000000000002</v>
       </c>
       <c r="K5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="M5">
         <v>3000000</v>
@@ -2221,7 +2127,7 @@
         <v>13</v>
       </c>
       <c r="O5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="P5" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
Fix #8177: Downloading questionnaire with Navigator results in file that is not importable (#8213)
* Fix #8211 Navigator download ignores internationalized labels and descriptions

* Fix metadataparser sets expressions even if they ar empty strings
</commit_message>
<xml_diff>
--- a/molgenis-platform-integration-tests/src/test/resources/xls/expectedDownloadResult.xlsx
+++ b/molgenis-platform-integration-tests/src/test/resources/xls/expectedDownloadResult.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bart\Documents\GitHub\molgenis\molgenis-platform-integration-tests\src\test\resources\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D20DDC6-25AD-41A2-A810-EB318D1D41CA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D0A29CD-6A94-4CB2-BD76-3B8FF9422924}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6910" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="112">
   <si>
     <t>name</t>
   </si>
@@ -64,6 +64,54 @@
   </si>
   <si>
     <t>backend</t>
+  </si>
+  <si>
+    <t>label-en</t>
+  </si>
+  <si>
+    <t>description-en</t>
+  </si>
+  <si>
+    <t>label-nl</t>
+  </si>
+  <si>
+    <t>description-nl</t>
+  </si>
+  <si>
+    <t>label-de</t>
+  </si>
+  <si>
+    <t>description-de</t>
+  </si>
+  <si>
+    <t>label-es</t>
+  </si>
+  <si>
+    <t>description-es</t>
+  </si>
+  <si>
+    <t>label-it</t>
+  </si>
+  <si>
+    <t>description-it</t>
+  </si>
+  <si>
+    <t>label-pt</t>
+  </si>
+  <si>
+    <t>description-pt</t>
+  </si>
+  <si>
+    <t>label-fr</t>
+  </si>
+  <si>
+    <t>description-fr</t>
+  </si>
+  <si>
+    <t>label-xx</t>
+  </si>
+  <si>
+    <t>description-xx</t>
   </si>
   <si>
     <t>test1</t>
@@ -666,7 +714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -730,13 +778,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -761,80 +809,110 @@
       <c r="H1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="H2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="H3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="H4" t="s">
         <v>6</v>
@@ -847,13 +925,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:W25"/>
+  <dimension ref="A1:AM25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -864,613 +942,661 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="I1" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="J1" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="K1" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="L1" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="M1" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="N1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="O1" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="P1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="Q1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="R1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="S1" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="T1" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="U1" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="V1" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="W1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="X1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="I2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="J2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="K2" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="M2" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="N2" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="W2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I3" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="J3" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="K3" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="L3" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="M3" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="N3" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="W3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="H4" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="I4" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="J4" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="K4" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="L4" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="M4" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="N4" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="W4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I5" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="J5" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="K5" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="L5" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="M5" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="N5" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="W5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I6" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="J6" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="L6" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="M6" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="N6" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="V6" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="W6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I7" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="J7" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="L7" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="M7" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="N7" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="W7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="G8" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I8" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="J8" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="L8" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="M8" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="N8" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="W8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="G9" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I9" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="J9" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="L9" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="M9" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="N9" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="W9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="G10" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="H10" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I10" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="J10" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="L10" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="M10" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="N10" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="O10" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="V10" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="W10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="G11" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="H11" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I11" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="J11" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="L11" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="M11" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="N11" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="W11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="G12" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="H12" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I12" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="J12" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="L12" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="M12" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="N12" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="W12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="G13" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="H13" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I13" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="J13" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="L13" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="M13" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="N13" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="W13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="G14" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="H14" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I14" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="J14" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="L14" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="M14" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="N14" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="W14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="G15" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="H15" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I15" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="J15" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="L15" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="M15" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="N15" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="W15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="G16" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="H16" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I16" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="J16" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="L16" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="M16" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="N16" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="W16" t="s">
         <v>6</v>
@@ -1478,37 +1604,37 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E17" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="G17" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="H17" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I17" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="J17" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="L17" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="M17" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="N17" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="V17" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="W17" t="s">
         <v>6</v>
@@ -1516,34 +1642,34 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E18" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="G18" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="H18" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I18" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="J18" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="L18" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="M18" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="N18" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="W18" t="s">
         <v>6</v>
@@ -1551,37 +1677,37 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E19" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="F19" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="G19" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="H19" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I19" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="J19" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="L19" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="M19" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="N19" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="W19" t="s">
         <v>6</v>
@@ -1589,37 +1715,37 @@
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="F20" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="G20" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="H20" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I20" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="J20" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="L20" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="M20" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="N20" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="W20" t="s">
         <v>6</v>
@@ -1627,37 +1753,37 @@
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="G21" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="H21" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I21" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="J21" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="L21" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="M21" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="N21" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="T21" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="W21" t="s">
         <v>6</v>
@@ -1665,34 +1791,34 @@
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="D22" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E22" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="G22" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="H22" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I22" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="J22" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="L22" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="M22" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="N22" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="W22" t="s">
         <v>6</v>
@@ -1700,37 +1826,37 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E23" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="G23" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="H23" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I23" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="J23" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="L23" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="M23" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="N23" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="P23" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="W23" t="s">
         <v>6</v>
@@ -1738,37 +1864,37 @@
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="D24" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="E24" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="G24" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="H24" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="I24" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="J24" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="K24" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="L24" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="M24" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="N24" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="W24" t="s">
         <v>6</v>
@@ -1776,37 +1902,37 @@
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D25" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="E25" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="G25" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="H25" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I25" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="J25" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="K25" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="L25" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="M25" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="N25" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="W25" t="s">
         <v>6</v>
@@ -1827,26 +1953,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1864,96 +1990,96 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="E1" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="F1" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="G1" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="H1" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="I1" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="J1" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="K1" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="L1" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="M1" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="N1" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="O1" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="P1" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="Q1" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="R1" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="S1" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="E2" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="F2" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="G2" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="H2" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="I2" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="J2">
         <v>0.123</v>
       </c>
       <c r="L2" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -1962,13 +2088,13 @@
         <v>10</v>
       </c>
       <c r="O2" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="P2" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="Q2" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="S2">
         <v>10</v>
@@ -1976,40 +2102,40 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="F3" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="G3" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="H3" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="I3" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="J3">
         <v>1.123</v>
       </c>
       <c r="K3" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="L3" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="M3">
         <v>1000000</v>
@@ -2018,13 +2144,13 @@
         <v>11</v>
       </c>
       <c r="O3" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="P3" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="Q3" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="S3">
         <v>11</v>
@@ -2032,37 +2158,37 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="E4" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="F4" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="G4" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="H4" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="I4" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="J4">
         <v>2.1230000000000002</v>
       </c>
       <c r="L4" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="M4">
         <v>2000000</v>
@@ -2071,13 +2197,13 @@
         <v>12</v>
       </c>
       <c r="O4" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="P4" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="Q4" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="S4">
         <v>12</v>
@@ -2085,40 +2211,40 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="E5" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="F5" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="G5" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="H5" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="I5" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="J5">
         <v>3.1230000000000002</v>
       </c>
       <c r="K5" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="L5" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="M5">
         <v>3000000</v>
@@ -2127,13 +2253,13 @@
         <v>13</v>
       </c>
       <c r="O5" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="P5" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="Q5" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="S5">
         <v>13</v>
@@ -2154,26 +2280,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: expose maxLength in EMX
</commit_message>
<xml_diff>
--- a/molgenis-platform-integration-tests/src/test/resources/xls/expectedDownloadResult.xlsx
+++ b/molgenis-platform-integration-tests/src/test/resources/xls/expectedDownloadResult.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fkelpin/git/molgenis2/molgenis-platform-integration-tests/src/test/resources/xls/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fkelpin/git/molgenis/molgenis-platform-integration-tests/src/test/resources/xls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290926C2-4167-4F4E-A644-0534E1C747B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D497109-0153-5846-A5A7-8E0D83962F49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34400" yWindow="-8220" windowWidth="28900" windowHeight="8200" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,8 @@
     <sheet name="pack_test1" sheetId="5" r:id="rId5"/>
     <sheet name="pack_refTest1" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -35,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="112">
   <si>
     <t>name</t>
   </si>
@@ -368,6 +363,9 @@
   </si>
   <si>
     <t>1985-08-12T06:12:13Z</t>
+  </si>
+  <si>
+    <t>maxLength</t>
   </si>
 </sst>
 </file>
@@ -933,18 +931,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AN25"/>
+  <dimension ref="A1:AO25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S2" sqref="S1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1026" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1000,73 +998,76 @@
         <v>49</v>
       </c>
       <c r="S1" t="s">
+        <v>111</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>52</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>53</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>4</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>54</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>12</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>13</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>14</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>15</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>16</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>17</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>18</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>19</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>20</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>21</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>22</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>23</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>24</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>25</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>26</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -1100,11 +1101,11 @@
       <c r="N2" t="s">
         <v>30</v>
       </c>
-      <c r="X2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="Y2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -1138,11 +1139,11 @@
       <c r="N3" t="s">
         <v>30</v>
       </c>
-      <c r="X3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="Y3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -1176,11 +1177,11 @@
       <c r="N4" t="s">
         <v>30</v>
       </c>
-      <c r="X4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="Y4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -1214,11 +1215,11 @@
       <c r="N5" t="s">
         <v>30</v>
       </c>
-      <c r="X5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="Y5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -1249,14 +1250,14 @@
       <c r="N6" t="s">
         <v>30</v>
       </c>
-      <c r="V6" t="s">
-        <v>57</v>
-      </c>
-      <c r="X6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="W6" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -1290,11 +1291,11 @@
       <c r="N7" t="s">
         <v>30</v>
       </c>
-      <c r="X7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="Y7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -1328,11 +1329,11 @@
       <c r="N8" t="s">
         <v>30</v>
       </c>
-      <c r="X8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="Y8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>67</v>
       </c>
@@ -1363,11 +1364,11 @@
       <c r="N9" t="s">
         <v>30</v>
       </c>
-      <c r="X9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="Y9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -1401,14 +1402,14 @@
       <c r="O10" t="s">
         <v>71</v>
       </c>
-      <c r="V10" t="s">
+      <c r="W10" t="s">
         <v>72</v>
       </c>
-      <c r="X10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="Y10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>73</v>
       </c>
@@ -1439,11 +1440,11 @@
       <c r="N11" t="s">
         <v>30</v>
       </c>
-      <c r="X11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="Y11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>75</v>
       </c>
@@ -1474,11 +1475,11 @@
       <c r="N12" t="s">
         <v>30</v>
       </c>
-      <c r="X12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="Y12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>77</v>
       </c>
@@ -1509,11 +1510,11 @@
       <c r="N13" t="s">
         <v>30</v>
       </c>
-      <c r="X13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="Y13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -1544,11 +1545,11 @@
       <c r="N14" t="s">
         <v>30</v>
       </c>
-      <c r="X14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="Y14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>81</v>
       </c>
@@ -1579,11 +1580,11 @@
       <c r="N15" t="s">
         <v>30</v>
       </c>
-      <c r="X15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="Y15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>83</v>
       </c>
@@ -1614,11 +1615,11 @@
       <c r="N16" t="s">
         <v>30</v>
       </c>
-      <c r="X16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -1649,14 +1650,14 @@
       <c r="N17" t="s">
         <v>30</v>
       </c>
-      <c r="V17" t="s">
+      <c r="W17" t="s">
         <v>87</v>
       </c>
-      <c r="X17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>88</v>
       </c>
@@ -1687,11 +1688,11 @@
       <c r="N18" t="s">
         <v>30</v>
       </c>
-      <c r="X18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>90</v>
       </c>
@@ -1725,11 +1726,11 @@
       <c r="N19" t="s">
         <v>30</v>
       </c>
-      <c r="X19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>92</v>
       </c>
@@ -1763,11 +1764,11 @@
       <c r="N20" t="s">
         <v>30</v>
       </c>
-      <c r="X20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>94</v>
       </c>
@@ -1798,14 +1799,14 @@
       <c r="N21" t="s">
         <v>30</v>
       </c>
-      <c r="T21" t="s">
+      <c r="U21" t="s">
         <v>85</v>
       </c>
-      <c r="X21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -1836,11 +1837,11 @@
       <c r="N22" t="s">
         <v>30</v>
       </c>
-      <c r="X22" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>97</v>
       </c>
@@ -1874,11 +1875,11 @@
       <c r="P23" t="s">
         <v>95</v>
       </c>
-      <c r="X23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -1912,11 +1913,11 @@
       <c r="N24" t="s">
         <v>30</v>
       </c>
-      <c r="X24" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -1950,7 +1951,7 @@
       <c r="N25" t="s">
         <v>30</v>
       </c>
-      <c r="X25" t="s">
+      <c r="Y25" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2007,7 +2008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>

</xml_diff>